<commit_message>
More Beta Updates - now with live aquisition
</commit_message>
<xml_diff>
--- a/SRUM_TEMPLATE2.xlsx
+++ b/SRUM_TEMPLATE2.xlsx
@@ -5,40 +5,53 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\host\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23070" windowHeight="9855" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23076" windowHeight="9852" firstSheet="11" activeTab="13"/>
   </bookViews>
   <sheets>
-    <sheet name="Network Usage" sheetId="1" r:id="rId1"/>
-    <sheet name="Application Resource Usage" sheetId="2" r:id="rId2"/>
-    <sheet name="Network Connections" sheetId="3" r:id="rId3"/>
-    <sheet name="Push Notification Data" sheetId="4" r:id="rId4"/>
-    <sheet name="Energy Usage LT" sheetId="5" r:id="rId5"/>
-    <sheet name="Energy Usage" sheetId="6" r:id="rId6"/>
-    <sheet name="Undocumented Windows 10 VM Data" sheetId="7" r:id="rId7"/>
-    <sheet name="Known SIDS" sheetId="8" r:id="rId8"/>
-    <sheet name="LUID Interfaces" sheetId="9" r:id="rId9"/>
+    <sheet name="Unknown4" sheetId="15" r:id="rId1"/>
+    <sheet name="Unknown1" sheetId="10" r:id="rId2"/>
+    <sheet name="Unknown3" sheetId="14" r:id="rId3"/>
+    <sheet name="Unknown2" sheetId="13" r:id="rId4"/>
+    <sheet name="Network Usage" sheetId="1" r:id="rId5"/>
+    <sheet name="Application Resource Usage" sheetId="2" r:id="rId6"/>
+    <sheet name="Network Connections" sheetId="3" r:id="rId7"/>
+    <sheet name="Push Notification Data" sheetId="4" r:id="rId8"/>
+    <sheet name="Energy Usage LT" sheetId="5" r:id="rId9"/>
+    <sheet name="Energy Usage" sheetId="6" r:id="rId10"/>
+    <sheet name="Undocumented Windows 10 VM Data" sheetId="7" r:id="rId11"/>
+    <sheet name="Lookup-Known SIDS" sheetId="8" r:id="rId12"/>
+    <sheet name="Lookup-LUID Interfaces" sheetId="9" r:id="rId13"/>
+    <sheet name="Lookup-ExampleNumNames" sheetId="16" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="H">#NAME?</definedName>
     <definedName name="I">#NAME?</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="9">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="10">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">#REF!</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="1">"Application Resource Usage"</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="5">"Energy Usage"</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="4">"Energy Usage"</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="2">"Network Connections"</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Network Usage"</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="3">"Push Notification Data"</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="6">"Undocumented Data"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="5">"Application Resource Usage"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="9">"Energy Usage"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="8">"Energy Usage"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="6">"Network Connections"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="4">"Network Usage"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="7">"Push Notification Data"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="10">"Undocumented Data"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="1">"Undocumented Data"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="3">"Undocumented Data"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="2">"Undocumented Data"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Undocumented Data"</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <webPublishing css="0" allowPng="1" codePage="1252"/>
@@ -46,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="435">
   <si>
     <t>AutoIncId</t>
   </si>
@@ -1171,6 +1184,186 @@
   </si>
   <si>
     <t>IF_TYPE_IPSWITCH</t>
+  </si>
+  <si>
+    <t>Flags</t>
+  </si>
+  <si>
+    <t>EndTime</t>
+  </si>
+  <si>
+    <t>DurationMS</t>
+  </si>
+  <si>
+    <t>SpanMS</t>
+  </si>
+  <si>
+    <t>TimelineEnd</t>
+  </si>
+  <si>
+    <t>InFocusTimeline</t>
+  </si>
+  <si>
+    <t>UserInputTimeline</t>
+  </si>
+  <si>
+    <t>CompRenderedTimeline</t>
+  </si>
+  <si>
+    <t>CompDirtiedTimeline</t>
+  </si>
+  <si>
+    <t>CompPropagatedTimeline</t>
+  </si>
+  <si>
+    <t>AudioInTimeline</t>
+  </si>
+  <si>
+    <t>AudioOutTimeline</t>
+  </si>
+  <si>
+    <t>CpuTimeline</t>
+  </si>
+  <si>
+    <t>DiskTimeline</t>
+  </si>
+  <si>
+    <t>NetworkTimeline</t>
+  </si>
+  <si>
+    <t>MBBTimeline</t>
+  </si>
+  <si>
+    <t>InFocusS</t>
+  </si>
+  <si>
+    <t>PSMForegroundS</t>
+  </si>
+  <si>
+    <t>UserInputS</t>
+  </si>
+  <si>
+    <t>CompRenderedS</t>
+  </si>
+  <si>
+    <t>CompDirtiedS</t>
+  </si>
+  <si>
+    <t>CompPropagatedS</t>
+  </si>
+  <si>
+    <t>AudioInS</t>
+  </si>
+  <si>
+    <t>AudioOutS</t>
+  </si>
+  <si>
+    <t>Cycles</t>
+  </si>
+  <si>
+    <t>CyclesBreakdown</t>
+  </si>
+  <si>
+    <t>CyclesAttr</t>
+  </si>
+  <si>
+    <t>CyclesAttrBreakdown</t>
+  </si>
+  <si>
+    <t>CyclesWOB</t>
+  </si>
+  <si>
+    <t>CyclesWOBBreakdown</t>
+  </si>
+  <si>
+    <t>DiskRaw</t>
+  </si>
+  <si>
+    <t>NetworkTailRaw</t>
+  </si>
+  <si>
+    <t>NetworkBytesRaw</t>
+  </si>
+  <si>
+    <t>MBBTailRaw</t>
+  </si>
+  <si>
+    <t>MBBBytesRaw</t>
+  </si>
+  <si>
+    <t>DisplayRequiredS</t>
+  </si>
+  <si>
+    <t>DisplayRequiredTimeline</t>
+  </si>
+  <si>
+    <t>KeyboardInputTimeline</t>
+  </si>
+  <si>
+    <t>KeyboardInputS</t>
+  </si>
+  <si>
+    <t>MouseInputS</t>
+  </si>
+  <si>
+    <t>StartTime</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>Metadata</t>
+  </si>
+  <si>
+    <t>Energy Data</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>{5C8CF1C7-7257-4F13-B223-970EF5939312}</t>
+  </si>
+  <si>
+    <t>{7ACBBAA3-D029-4BE4-9A7A-0885927F1D8F}</t>
+  </si>
+  <si>
+    <t>{B6D82AF1-F780-4E17-8077-6CB9AD8A6FC4}</t>
+  </si>
+  <si>
+    <t>{DA73FB89-2BEA-4DDC-86B8-6E048C6DA477}</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>Two</t>
+  </si>
+  <si>
+    <t>Three</t>
+  </si>
+  <si>
+    <t>Four</t>
+  </si>
+  <si>
+    <t>Five</t>
+  </si>
+  <si>
+    <t>Six</t>
+  </si>
+  <si>
+    <t>Seven</t>
+  </si>
+  <si>
+    <t>Eight</t>
+  </si>
+  <si>
+    <t>Nine</t>
+  </si>
+  <si>
+    <t>lookup-ExampleNumNames</t>
+  </si>
+  <si>
+    <t>Zero</t>
   </si>
 </sst>
 </file>
@@ -1552,120 +1745,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFA13"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" style="1" customWidth="1"/>
-    <col min="11" max="16381" width="9.140625" style="1" hidden="1"/>
-    <col min="16382" max="16384" width="11.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="22" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="22" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" style="22" customWidth="1"/>
+    <col min="5" max="8" width="9.109375" style="22" customWidth="1"/>
+    <col min="9" max="16383" width="9.109375" style="22"/>
+    <col min="16384" max="16384" width="29.109375" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="2" t="s">
-        <v>51</v>
+    <row r="1" spans="1:5">
+      <c r="A1" s="23" t="s">
+        <v>423</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:5" customFormat="1">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>7</v>
+      <c r="E2" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:5">
+      <c r="B3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>54</v>
-      </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="4" t="s">
+    <row r="4" spans="1:5">
+      <c r="A4" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="B13" s="2" t="s">
-        <v>63</v>
+      <c r="E4" s="24" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1675,592 +1819,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="39.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="26.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="31.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="28" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="5" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="B3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
-      <c r="A4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="S4" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" cellComments="asDisplayed"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="28.28515625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="8" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="B3" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="25" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="9"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="H9" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="I9" s="9"/>
-    </row>
-  </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" cellComments="asDisplayed" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="12" customWidth="1"/>
-    <col min="4" max="4" width="22" style="12" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" style="12" customWidth="1"/>
-    <col min="6" max="6" width="37.85546875" style="12" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" style="12" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="12" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="B3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" cellComments="asDisplayed"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFB4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="41.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="16382" width="9.140625" style="15" hidden="1"/>
-    <col min="16383" max="16384" width="9.140625" style="16" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" s="17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="K2" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="L2" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="M2" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="N2" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="O2" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="P2" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="B3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="M4" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="N4" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="O4" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="P4" s="18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" cellComments="asDisplayed"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="24" style="19" customWidth="1"/>
-    <col min="2" max="6" width="9.140625" style="19"/>
-    <col min="7" max="7" width="22.85546875" style="19" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" style="19" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="19"/>
+    <col min="2" max="6" width="9.109375" style="19"/>
+    <col min="7" max="7" width="22.88671875" style="19" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" style="19" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16384">
@@ -35106,22 +34681,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="22" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="22" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="22" customWidth="1"/>
-    <col min="5" max="8" width="9.140625" style="22" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="22" hidden="1"/>
+    <col min="1" max="1" width="9.109375" style="22" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="22" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" style="22" customWidth="1"/>
+    <col min="5" max="8" width="9.109375" style="22" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="22" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -35181,15 +34756,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -35780,13 +35353,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B145"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1">
@@ -36951,4 +36526,1148 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>434</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AR4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="9.109375" style="22" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="22" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" style="22" customWidth="1"/>
+    <col min="5" max="8" width="9.109375" style="22" customWidth="1"/>
+    <col min="9" max="16383" width="9.109375" style="22"/>
+    <col min="16384" max="16384" width="29.109375" style="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:44">
+      <c r="A1" s="23" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" customFormat="1">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>375</v>
+      </c>
+      <c r="F2" t="s">
+        <v>376</v>
+      </c>
+      <c r="G2" t="s">
+        <v>377</v>
+      </c>
+      <c r="H2" t="s">
+        <v>378</v>
+      </c>
+      <c r="I2" t="s">
+        <v>379</v>
+      </c>
+      <c r="J2" t="s">
+        <v>380</v>
+      </c>
+      <c r="K2" t="s">
+        <v>381</v>
+      </c>
+      <c r="L2" t="s">
+        <v>382</v>
+      </c>
+      <c r="M2" t="s">
+        <v>383</v>
+      </c>
+      <c r="N2" t="s">
+        <v>384</v>
+      </c>
+      <c r="O2" t="s">
+        <v>385</v>
+      </c>
+      <c r="P2" t="s">
+        <v>386</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>387</v>
+      </c>
+      <c r="R2" t="s">
+        <v>388</v>
+      </c>
+      <c r="S2" t="s">
+        <v>389</v>
+      </c>
+      <c r="T2" t="s">
+        <v>390</v>
+      </c>
+      <c r="U2" t="s">
+        <v>391</v>
+      </c>
+      <c r="V2" t="s">
+        <v>392</v>
+      </c>
+      <c r="W2" t="s">
+        <v>393</v>
+      </c>
+      <c r="X2" t="s">
+        <v>394</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>395</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>396</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>397</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>398</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>399</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>400</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>401</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>402</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>403</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>404</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>405</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>406</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>407</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>408</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>409</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>410</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>411</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>412</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>413</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44">
+      <c r="B3" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:44">
+      <c r="A4" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" cellComments="asDisplayed"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="9.109375" style="22" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="22" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" style="22" customWidth="1"/>
+    <col min="5" max="8" width="9.109375" style="22" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="22" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="23" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" customFormat="1">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>417</v>
+      </c>
+      <c r="F2" t="s">
+        <v>418</v>
+      </c>
+      <c r="G2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="24"/>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" cellComments="asDisplayed"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="9.109375" style="22" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="22" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" style="22" customWidth="1"/>
+    <col min="5" max="8" width="9.109375" style="22" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="22" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="23" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" customFormat="1">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>375</v>
+      </c>
+      <c r="F2" t="s">
+        <v>415</v>
+      </c>
+      <c r="G2" t="s">
+        <v>376</v>
+      </c>
+      <c r="H2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="B3" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>375</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" cellComments="asDisplayed"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:XFA13"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="39.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.109375" style="1" customWidth="1"/>
+    <col min="11" max="16381" width="9.109375" style="1" hidden="1"/>
+    <col min="16382" max="16384" width="11.109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="B13" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" cellComments="asDisplayed"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="39.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="26.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.109375" style="5" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="B3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" cellComments="asDisplayed"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="28.33203125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="8" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="B3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="9"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="H9" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="9"/>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" cellComments="asDisplayed" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="9.109375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" style="12" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="22" style="12" customWidth="1"/>
+    <col min="5" max="5" width="28.5546875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="37.88671875" style="12" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="12" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="12" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" cellComments="asDisplayed"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:XFB4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="41.5546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.88671875" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.88671875" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" style="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="16382" width="9.109375" style="15" hidden="1"/>
+    <col min="16383" max="16384" width="9.109375" style="16" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="B3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="O4" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="P4" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" cellComments="asDisplayed"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix ConnectedTime on Network Connection Tab
</commit_message>
<xml_diff>
--- a/SRUM_TEMPLATE2.xlsx
+++ b/SRUM_TEMPLATE2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\host\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23076" windowHeight="9852" firstSheet="11" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23070" windowHeight="9855" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Unknown4" sheetId="15" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="436">
   <si>
     <t>AutoIncId</t>
   </si>
@@ -1364,6 +1364,9 @@
   </si>
   <si>
     <t>Zero</t>
+  </si>
+  <si>
+    <t>seconds</t>
   </si>
 </sst>
 </file>
@@ -1751,15 +1754,15 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="22" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" style="22" customWidth="1"/>
-    <col min="5" max="8" width="9.109375" style="22" customWidth="1"/>
-    <col min="9" max="16383" width="9.109375" style="22"/>
-    <col min="16384" max="16384" width="29.109375" style="22" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="22" customWidth="1"/>
+    <col min="5" max="8" width="9.140625" style="22" customWidth="1"/>
+    <col min="9" max="16383" width="9.140625" style="22"/>
+    <col min="16384" max="16384" width="29.140625" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1827,15 +1830,15 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24" style="19" customWidth="1"/>
-    <col min="2" max="6" width="9.109375" style="19"/>
-    <col min="7" max="7" width="22.88671875" style="19" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" style="19" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37.109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="19"/>
+    <col min="2" max="6" width="9.140625" style="19"/>
+    <col min="7" max="7" width="22.85546875" style="19" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" style="19" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16384">
@@ -34689,14 +34692,14 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="22" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" style="22" customWidth="1"/>
-    <col min="5" max="8" width="9.109375" style="22" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="22" hidden="1"/>
+    <col min="1" max="1" width="9.140625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="22" customWidth="1"/>
+    <col min="5" max="8" width="9.140625" style="22" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="22" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -34762,7 +34765,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -35361,7 +35364,7 @@
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1">
@@ -36532,11 +36535,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1">
@@ -36629,15 +36632,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="22" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" style="22" customWidth="1"/>
-    <col min="5" max="8" width="9.109375" style="22" customWidth="1"/>
-    <col min="9" max="16383" width="9.109375" style="22"/>
-    <col min="16384" max="16384" width="29.109375" style="22" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="22" customWidth="1"/>
+    <col min="5" max="8" width="9.140625" style="22" customWidth="1"/>
+    <col min="9" max="16383" width="9.140625" style="22"/>
+    <col min="16384" max="16384" width="29.140625" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44">
@@ -36822,14 +36825,14 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="22" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" style="22" customWidth="1"/>
-    <col min="5" max="8" width="9.109375" style="22" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="22" hidden="1"/>
+    <col min="1" max="1" width="9.140625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="22" customWidth="1"/>
+    <col min="5" max="8" width="9.140625" style="22" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="22" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -36899,14 +36902,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="22" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" style="22" customWidth="1"/>
-    <col min="5" max="8" width="9.109375" style="22" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="22" hidden="1"/>
+    <col min="1" max="1" width="9.140625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="22" customWidth="1"/>
+    <col min="5" max="8" width="9.140625" style="22" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="22" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -36983,20 +36986,20 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.109375" style="1" customWidth="1"/>
-    <col min="11" max="16381" width="9.109375" style="1" hidden="1"/>
-    <col min="16382" max="16384" width="11.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" style="1" customWidth="1"/>
+    <col min="11" max="16381" width="9.140625" style="1" hidden="1"/>
+    <col min="16382" max="16384" width="11.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -37111,27 +37114,27 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="26.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="26.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="28" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="31.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="28" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.109375" style="5" hidden="1"/>
+    <col min="20" max="16384" width="9.140625" style="5" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -37279,23 +37282,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="8" hidden="1"/>
+    <col min="1" max="1" width="28.28515625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="8" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -37350,6 +37353,9 @@
       </c>
       <c r="F3" s="9" t="s">
         <v>11</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>435</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>31</v>
@@ -37438,16 +37444,16 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" style="12" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="12" customWidth="1"/>
     <col min="4" max="4" width="22" style="12" customWidth="1"/>
-    <col min="5" max="5" width="28.5546875" style="12" customWidth="1"/>
-    <col min="6" max="6" width="37.88671875" style="12" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" style="12" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="12" hidden="1"/>
+    <col min="5" max="5" width="28.5703125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="37.85546875" style="12" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" style="12" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="12" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -37527,26 +37533,26 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.5546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.88671875" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" style="15" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="15" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="16382" width="9.109375" style="15" hidden="1"/>
-    <col min="16383" max="16384" width="9.109375" style="16" hidden="1"/>
+    <col min="16" max="16" width="17.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="16382" width="9.140625" style="15" hidden="1"/>
+    <col min="16383" max="16384" width="9.140625" style="16" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">

</xml_diff>